<commit_message>
In Excel Sheet as weel now faculty needs permission for inputting the marks.
</commit_message>
<xml_diff>
--- a/Sem 1.xlsx
+++ b/Sem 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1392,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2357,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>